<commit_message>
rh_email added in element table (i.e) no need to import contacts to send mail
</commit_message>
<xml_diff>
--- a/data/sample1.xlsx
+++ b/data/sample1.xlsx
@@ -709,7 +709,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -719,10 +719,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1066,8 +1066,8 @@
     <hyperlink ref="N5:N6" r:id="rId7" display="\\10.1.1.100\copyediting\04-Rights&amp;Media\02_JBL\Volsko_17364-1\02_Research\Photo\Photo Research\Volsko_2e_Research options"/>
     <hyperlink ref="N7" r:id="rId8"/>
     <hyperlink ref="I2" r:id="rId9"/>
-    <hyperlink ref="K4:K7" r:id="rId10" display="sulthanaofficial111@gmail.com"/>
-    <hyperlink ref="N4" r:id="rId11"/>
+    <hyperlink ref="N4" r:id="rId10"/>
+    <hyperlink ref="K4:K7" r:id="rId11" display="sulthanaofficial111@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId12"/>

</xml_diff>

<commit_message>
mail configuration for test
</commit_message>
<xml_diff>
--- a/data/sample1.xlsx
+++ b/data/sample1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="825" windowWidth="17520" windowHeight="13200"/>
+    <workbookView xWindow="-15" yWindow="2970" windowWidth="12750" windowHeight="3030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -709,7 +709,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -719,10 +719,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
+      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>